<commit_message>
Update profile creating tool.xlsx
</commit_message>
<xml_diff>
--- a/SecondKeyboard/iCue/profile creating tool.xlsx
+++ b/SecondKeyboard/iCue/profile creating tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Woong\Documents\GitHub\Scripts\SecondKeyboard\iCue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEECF55-85E0-44FF-8A7F-54CE9B7E6447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B897164-2B2E-4B91-9580-EE581B993997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2B087225-0969-45CE-ABD6-9F0C4354DA0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B087225-0969-45CE-ABD6-9F0C4354DA0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="365">
   <si>
     <t>&lt;value</t>
   </si>
@@ -1910,24 +1910,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF660FC2-EEA2-4848-8FC4-144E4F2F697C}">
-  <dimension ref="A1:AG113"/>
+  <dimension ref="A1:AG144"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78:C113"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A146" sqref="A130:AI146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="4"/>
-    <col min="20" max="20" width="9.140625" style="3"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="24.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" style="4"/>
+    <col min="20" max="20" width="9.109375" style="3"/>
+    <col min="21" max="21" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>&lt;value2&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483663&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro1&lt;/name&gt; &lt;id&gt;{414cf73f-2b35-4180-bc9d-9c250d0fb535}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;F13&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value2&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="str">
         <f>A2</f>
         <v>&lt;value</v>
@@ -2066,7 +2066,7 @@
         <v>&lt;value3&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483664&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro2&lt;/name&gt; &lt;id&gt;{32d6b8d2-6c92-0214-3be7-6637c378521c}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;F13&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value3&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="str">
         <f t="shared" ref="A4:A9" si="2">A3</f>
         <v>&lt;value</v>
@@ -2128,7 +2128,7 @@
         <v>&lt;value4&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483665&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro3&lt;/name&gt; &lt;id&gt;{8429e02c-2af0-718a-0b67-0e6a51236d1f}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;F13&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value4&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;value</v>
@@ -2190,7 +2190,7 @@
         <v>&lt;value5&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483666&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro4&lt;/name&gt; &lt;id&gt;{74eb7793-1083-4fb6-50d6-8bb657a61168}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F13&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value5&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;value</v>
@@ -2252,7 +2252,7 @@
         <v>&lt;value6&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483667&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro5&lt;/name&gt; &lt;id&gt;{ecc7938f-59da-89a3-6bbf-3644105830f5}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;F13&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value6&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;value</v>
@@ -2314,7 +2314,7 @@
         <v>&lt;value7&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483668&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro6&lt;/name&gt; &lt;id&gt;{d46732d4-1d4b-049e-1881-8b9125b63a88}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;F13&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value7&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;value</v>
@@ -2376,7 +2376,7 @@
         <v>&lt;value8&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483669&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro7&lt;/name&gt; &lt;id&gt;{1e4c071e-a13e-93cd-4c88-a1c80a7c8dde}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F13&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value8&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;value</v>
@@ -2438,7 +2438,7 @@
         <v>&lt;value9&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483670&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro8&lt;/name&gt; &lt;id&gt;{295c8f14-a777-9611-1623-c37c2bdf6ff0}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;F13&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value9&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" ref="A10:A17" si="9">A9</f>
         <v>&lt;value</v>
@@ -2503,7 +2503,7 @@
         <v>&lt;value10&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483671&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro9&lt;/name&gt; &lt;id&gt;{7e353507-60bd-2043-04c3-e8b6480265bb}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;F14&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value10&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2568,7 +2568,7 @@
         <v>&lt;value11&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483672&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro10&lt;/name&gt; &lt;id&gt;{2805a72c-76a4-64e5-38fa-27ed51de1c42}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;F14&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value11&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2633,7 +2633,7 @@
         <v>&lt;value12&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483673&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro11&lt;/name&gt; &lt;id&gt;{e011abfe-5e7e-54a2-9ee2-f826f2775f55}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;F14&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value12&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2698,7 +2698,7 @@
         <v>&lt;value13&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483674&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro12&lt;/name&gt; &lt;id&gt;{bac2cf0f-598f-1ac8-7e19-d517ca032d41}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F14&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value13&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2763,7 +2763,7 @@
         <v>&lt;value14&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483675&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro13&lt;/name&gt; &lt;id&gt;{ece64916-3996-9483-4524-777ec9629dc3}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;F14&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value14&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2828,7 +2828,7 @@
         <v>&lt;value15&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483676&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro14&lt;/name&gt; &lt;id&gt;{ed1abd5a-a753-0d2b-89a8-a24fc9511d78}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;F14&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value15&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2893,7 +2893,7 @@
         <v>&lt;value16&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483677&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro15&lt;/name&gt; &lt;id&gt;{c64b6fb2-3305-66fd-3b5f-a8e3a9d217c5}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F14&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value16&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="9"/>
         <v>&lt;value</v>
@@ -2958,7 +2958,7 @@
         <v>&lt;value17&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483678&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro16&lt;/name&gt; &lt;id&gt;{f5751d48-78b1-8b05-9a20-ec741b8ea3f8}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;F14&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value17&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" ref="A18:A81" si="24">A17</f>
         <v>&lt;value</v>
@@ -3023,7 +3023,7 @@
         <v>&lt;value18&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483679&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro17&lt;/name&gt; &lt;id&gt;{3c15809f-9310-5934-3305-f56ad8877d01}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;F15&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value18&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3091,7 +3091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3156,7 +3156,7 @@
         <v>&lt;value20&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483681&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro19&lt;/name&gt; &lt;id&gt;{d7ca59ea-7b46-827e-2622-20cae0370699}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;F15&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value20&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3221,7 +3221,7 @@
         <v>&lt;value21&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483682&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro20&lt;/name&gt; &lt;id&gt;{f5281981-7eee-7dd9-788a-76014b183eb4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F15&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value21&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3286,7 +3286,7 @@
         <v>&lt;value22&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483683&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro21&lt;/name&gt; &lt;id&gt;{5467515c-6842-1fd7-588e-c1f5cd01454f}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;F15&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value22&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3354,7 +3354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3422,7 +3422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3490,7 +3490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3558,7 +3558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3623,7 +3623,7 @@
         <v>&lt;value27&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483688&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro26&lt;/name&gt; &lt;id&gt;{4b0f6be7-33f0-2053-3601-c78159794ebe}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;F16&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value27&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3697,7 +3697,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3771,7 +3771,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3845,7 +3845,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3919,7 +3919,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -3993,7 +3993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4067,7 +4067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4141,7 +4141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4215,7 +4215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4280,7 +4280,7 @@
         <v>&lt;value36&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483697&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro35&lt;/name&gt; &lt;id&gt;{472568e4-49ac-9cf3-951a-06bd68419d31}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;F17&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value36&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4345,7 +4345,7 @@
         <v>&lt;value37&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483698&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro36&lt;/name&gt; &lt;id&gt;{fc308fc4-653f-776c-877a-e4ddf54501e7}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;F17&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value37&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4410,7 +4410,7 @@
         <v>&lt;value38&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483699&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro37&lt;/name&gt; &lt;id&gt;{4565bad7-839a-2d75-3ab1-1927d14050da}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;F17&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value38&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4481,7 +4481,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4547,7 +4547,7 @@
       </c>
       <c r="W40" t="str">
         <f t="shared" ref="W40:W101" ca="1" si="78">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,42949),4),"-",DEC2HEX(RANDBETWEEN(0,4294967295),8),DEC2HEX(RANDBETWEEN(0,42949),4)))</f>
-        <v>09d5dab5-4681-69df-5d65-8ff5e7b64c85</v>
+        <v>a7b8e3e5-3f9e-0538-2597-828fe53b204f</v>
       </c>
       <c r="AE40" t="s">
         <v>57</v>
@@ -4556,7 +4556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="W41" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>e0870fe2-a546-6ad7-225c-cb33e7e444b1</v>
+        <v>10a600ce-32b0-9d06-4973-b9103abc13af</v>
       </c>
       <c r="AE41" t="s">
         <v>58</v>
@@ -4631,7 +4631,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="W42" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>02edba17-1073-78c8-79e7-c96173309fdc</v>
+        <v>7e9d49ab-7cd8-6474-7a2d-6190ecee7e2e</v>
       </c>
       <c r="AE42" t="s">
         <v>59</v>
@@ -4706,7 +4706,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4772,7 +4772,7 @@
       </c>
       <c r="W43" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>17290348-2ece-4bd3-3bc3-135702eb7682</v>
+        <v>7f17eceb-20aa-8362-8856-b377062c53e4</v>
       </c>
       <c r="AE43" t="s">
         <v>60</v>
@@ -4781,7 +4781,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="W44" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>c95365a1-4541-9ef4-5437-b6b768496caa</v>
+        <v>258c22e8-3913-5d08-943b-1770973a5775</v>
       </c>
       <c r="AE44" t="s">
         <v>61</v>
@@ -4856,7 +4856,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="W45" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>92bc0804-7e5d-474b-06fd-6af5b965a442</v>
+        <v>8d4ee2bb-97fe-45c0-76d4-243bf4d957a7</v>
       </c>
       <c r="AE45" t="s">
         <v>62</v>
@@ -4931,7 +4931,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="W46" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>8797b516-83a6-2dec-11f7-eb9b1bff78c2</v>
+        <v>7c38bd34-8573-79f5-1db4-f43cb9f19f77</v>
       </c>
       <c r="AE46" t="s">
         <v>63</v>
@@ -5006,7 +5006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5072,10 +5072,10 @@
       </c>
       <c r="W47" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>8f54bbce-3eef-30b9-8cd4-f989dc2921c8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+        <v>f01b4c7f-0614-66b7-811d-47c7259d11ff</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5141,10 +5141,10 @@
       </c>
       <c r="W48" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>f0b4cb45-44ec-7b8f-0d34-7b6d3be0130a</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0a5ba86a-5338-82d8-6a84-2d72b94428d9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5210,10 +5210,10 @@
       </c>
       <c r="W49" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>f3e6cdef-a135-1bc5-369e-6d53712751c1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+        <v>d355a106-876a-4ccd-7cae-176ffcf00023</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5279,10 +5279,10 @@
       </c>
       <c r="W50" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>ea441322-248d-47bc-1c67-b30e31c19dfc</v>
-      </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2c241888-74bc-2b75-7ff2-e809eb4f950d</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5348,10 +5348,10 @@
       </c>
       <c r="W51" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>b2318fe9-7678-18e2-70da-6aedc187281a</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+        <v>632fce18-43a7-0ac4-4390-88a2f821a739</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5417,10 +5417,10 @@
       </c>
       <c r="W52" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>13934c7c-4e4f-a400-5681-c96676de2af3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+        <v>41becca8-4b3b-0054-9082-3d1bf33d4b70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5486,10 +5486,10 @@
       </c>
       <c r="W53" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>70115a38-9dd9-44e4-0d16-e304c8e0182f</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+        <v>dacb553b-3c48-084f-16cf-f2d500ff7e72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5555,10 +5555,10 @@
       </c>
       <c r="W54" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>ce1414ed-6e84-96ad-645a-b27957f64b48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+        <v>6d24742b-3598-3857-1035-a6711beb8dfc</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5624,10 +5624,10 @@
       </c>
       <c r="W55" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>de458e87-1563-0cfa-5c89-42f6cb160c10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+        <v>ea917f1c-2ee8-853c-7b42-47cf53a68a28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5693,10 +5693,10 @@
       </c>
       <c r="W56" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>d771a76a-8e31-2f82-97e7-f0a1be28571a</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+        <v>28bbfca3-91c1-1c89-936e-c9e0fa951b27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5762,10 +5762,10 @@
       </c>
       <c r="W57" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>3dea747b-4c51-0753-4c6b-afefc3c81892</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+        <v>43b49881-29c1-20ea-4bfa-6134cbdf8e22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5831,10 +5831,10 @@
       </c>
       <c r="W58" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>2f804201-3275-34c7-9f92-c32cec341db4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+        <v>7e51fa0d-2dcf-9881-8598-a3be88d0122c</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5900,10 +5900,10 @@
       </c>
       <c r="W59" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>747c4efa-5ebd-13c0-1be1-5fa17c912b4e</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4ef658b2-8db1-1e0a-4e3e-f46436f38591</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -5969,10 +5969,10 @@
       </c>
       <c r="W60" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>cc2d8a2d-516d-9323-24e4-bdeb11bd4caa</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+        <v>01510098-3c88-756f-9dbb-ce0e96bb35b9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6038,10 +6038,10 @@
       </c>
       <c r="W61" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>1ed0994c-1263-5ed7-3a9c-1ae204c22eb5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+        <v>30438d4a-3e1b-073b-3530-7e4dc70f457d</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6107,10 +6107,10 @@
       </c>
       <c r="W62" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>b7a03531-3075-0b53-4c0c-7d7e350f96c6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+        <v>b53ad63b-8603-8c8b-57cc-366993c44024</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6176,10 +6176,10 @@
       </c>
       <c r="W63" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>37edc73c-3fc9-8902-6b60-8c06c5e04b99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+        <v>860d436b-71fb-0c48-53d5-ef56b2fc4db3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6245,10 +6245,10 @@
       </c>
       <c r="W64" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>bd1c95a5-5b2d-8bcc-6239-c4629154771f</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2bbcb8ff-27b5-0ff9-a0fe-17b8d7dfa794</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6314,10 +6314,10 @@
       </c>
       <c r="W65" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>62e1da11-a504-9f74-95c6-6def49444f79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+        <v>25893c67-071b-7bd5-0ad2-8adcbcf3484d</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6383,10 +6383,10 @@
       </c>
       <c r="W66" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>f22146da-2b38-1249-37fc-42f07b203a41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0b812160-59b6-0bf1-5a1c-f03b428f44b6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6452,10 +6452,10 @@
       </c>
       <c r="W67" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>0b5efdb3-2b87-8fe2-4679-ef16d4e5a643</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+        <v>faaff690-2e6d-a012-7f3d-0e24289a7c85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6521,10 +6521,10 @@
       </c>
       <c r="W68" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>8c9fc893-7de1-1977-7356-2341f5584bfa</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1ed2b351-a318-81f6-3daa-207aac4b2e2a</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6590,10 +6590,10 @@
       </c>
       <c r="W69" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>5be078c8-5808-a2f9-4642-12d3c7ea7c44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+        <v>5a4cd48e-3917-54c6-903a-e332dbf89275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6659,10 +6659,10 @@
       </c>
       <c r="W70" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>48261dbe-7eac-2214-9481-55db082e8fc1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+        <v>5d88daf7-66be-368e-a3cf-9aa699d90a90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6728,10 +6728,10 @@
       </c>
       <c r="W71" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>ea0e6706-15e1-660c-5385-347884306f45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2cb5e4e9-4ddb-2218-7cbd-565d6af87fc4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6797,10 +6797,10 @@
       </c>
       <c r="W72" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>7aa61f62-9829-5421-75dd-7ae44d269832</v>
-      </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+        <v>ffbe16d9-38b4-0ab7-44a7-81dc46760824</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6866,10 +6866,10 @@
       </c>
       <c r="W73" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>24d0885c-a494-6aea-a11b-e9877c52031b</v>
-      </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+        <v>f7d7e676-2bc3-8103-8219-331a82178480</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6935,10 +6935,10 @@
       </c>
       <c r="W74" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>486569d3-0fef-333e-282c-f54c874a491c</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+        <v>e6a3da44-1c82-2dcf-8b02-9f4deac10d43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -6995,7 +6995,7 @@
         <v>1</v>
       </c>
       <c r="Q75">
-        <f t="shared" ref="Q75:Q113" si="150">Q67+1</f>
+        <f t="shared" ref="Q75:Q138" si="150">Q67+1</f>
         <v>22</v>
       </c>
       <c r="T75" s="3" t="str">
@@ -7004,10 +7004,10 @@
       </c>
       <c r="W75" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>08772f42-59f6-3e19-33f0-f76d443a2845</v>
-      </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+        <v>d7cbd69b-0983-33ce-6a5e-951068416545</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7073,10 +7073,10 @@
       </c>
       <c r="W76" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>1260363b-5802-9bde-814d-92eab442485e</v>
-      </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1865ff6b-288b-1425-61a3-b5e565574acd</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7142,10 +7142,10 @@
       </c>
       <c r="W77" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>900db94a-7d9e-198a-5b8d-155eb7c60682</v>
-      </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+        <v>61e29d29-0d4e-6eb3-3b9a-2895f4c38d8c</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7211,10 +7211,10 @@
       </c>
       <c r="W78" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>9a2974d4-5691-98d6-241a-a51ee57d3642</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+        <v>33e4c6e3-7b99-0fd2-92dd-af4913e9797f</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7280,10 +7280,10 @@
       </c>
       <c r="W79" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>781bb8ca-737c-2144-8b0a-8244031d7644</v>
-      </c>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+        <v>7d2f6e73-49de-493c-3860-0a0566690f47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7349,10 +7349,10 @@
       </c>
       <c r="W80" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>ebea0569-4c4d-82a3-6eee-78f4b52b6e28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+        <v>6bcb6d6b-2de7-6804-9c21-4936e7bea4e5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="str">
         <f t="shared" si="24"/>
         <v>&lt;value</v>
@@ -7418,10 +7418,10 @@
       </c>
       <c r="W81" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>7ee68868-3fd8-a595-83ef-ac503bd09a7e</v>
-      </c>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+        <v>fdfafa7e-7d0c-7e5e-3692-98023bf42e7d</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="str">
         <f t="shared" ref="A82:A107" si="163">A81</f>
         <v>&lt;value</v>
@@ -7431,7 +7431,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="1" t="str">
-        <f t="shared" ref="C82:C113" si="165">C81</f>
+        <f t="shared" ref="C82:C144" si="165">C81</f>
         <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
       </c>
       <c r="D82">
@@ -7487,10 +7487,10 @@
       </c>
       <c r="W82" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>d47635f5-05ff-40ee-17da-23df7d1b5a7d</v>
-      </c>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+        <v>ec6810c5-92dd-5c10-47b9-18ef0774a76c</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7556,10 +7556,10 @@
       </c>
       <c r="W83" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>0189cc99-2983-68e9-2cf7-bc4f5cef1c09</v>
-      </c>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+        <v>b033901d-272a-54db-7a1b-947fc7b56790</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7625,10 +7625,10 @@
       </c>
       <c r="W84" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>bbebf6db-56b1-33d7-a46b-bbddb98716da</v>
-      </c>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0c47c817-6aec-335d-224a-d9d4529d0274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7694,10 +7694,10 @@
       </c>
       <c r="W85" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>72755af4-8916-87d9-825c-0d01839b5245</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+        <v>c60fde04-5485-72c0-0bd7-e8df9d4e2b87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7763,10 +7763,10 @@
       </c>
       <c r="W86" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>a029b04b-739a-2ec9-4a2c-fecfd5e9796d</v>
-      </c>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+        <v>7c029f2b-5243-22af-2d40-2df4d44d712a</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7832,10 +7832,10 @@
       </c>
       <c r="W87" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>7b4b34e9-19d8-4d6d-3076-37ce695862e5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+        <v>528f43f1-879f-1395-4e43-b336d60d2227</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7901,10 +7901,10 @@
       </c>
       <c r="W88" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>87df4581-0f0e-59f7-6755-d7f353c6750a</v>
-      </c>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0772c022-0fe1-37bc-0696-67e391ca854d</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -7970,10 +7970,10 @@
       </c>
       <c r="W89" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>f98a7593-5033-586f-3926-da068cc82e72</v>
-      </c>
-    </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+        <v>93ad5114-39a8-3fa8-a24a-2c5ca8dd7bdf</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8039,10 +8039,10 @@
       </c>
       <c r="W90" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>fa43e1d8-2f8d-8e22-90f9-8e56f7cd8229</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+        <v>5970b3b9-4ea6-4c22-3110-c38435ec1c6a</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8108,10 +8108,10 @@
       </c>
       <c r="W91" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>94b2cfd8-01b9-792d-1032-6993843644f3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+        <v>9cfec060-4bdb-32c7-9a55-a52a924244a3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8177,10 +8177,10 @@
       </c>
       <c r="W92" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>22e55c1c-09fd-9cc1-32e2-8a62bf3687d8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0170d6e8-2d50-76de-5ad0-4d39255236bf</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8246,10 +8246,10 @@
       </c>
       <c r="W93" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>851f238d-4715-10a0-4bb2-66c2af315d44</v>
-      </c>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+        <v>7bb7103f-1fe4-4d73-3df4-d9ba296c3f31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8315,10 +8315,10 @@
       </c>
       <c r="W94" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>896e09ee-178c-5592-5525-61d94b51a6c9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+        <v>cffb49f5-1dd9-61bb-3cf9-e13c0a9a99c4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8384,10 +8384,10 @@
       </c>
       <c r="W95" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>20fef932-2154-0109-4631-72362f70985c</v>
-      </c>
-    </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+        <v>ac0277ae-617c-8f68-910e-9e4c56184fcf</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8453,10 +8453,10 @@
       </c>
       <c r="W96" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>3befb55b-a006-0d42-654d-4f42ef536d11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+        <v>3c86e114-890a-2835-62ae-54bdff8b8949</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8522,10 +8522,10 @@
       </c>
       <c r="W97" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>7c591513-82a0-542b-8729-6ceb5a54592b</v>
-      </c>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+        <v>53edf2a2-9765-3165-804f-c680ab45733b</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8590,10 +8590,10 @@
       </c>
       <c r="W98" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>4c64fdfe-27b4-1b79-6232-2a82b0f33b24</v>
-      </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+        <v>67ae7d74-a28d-9542-8e0d-737a63de2b91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8658,10 +8658,10 @@
       </c>
       <c r="W99" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>19d2a487-3e3d-99ef-0e43-ca2a093a40fa</v>
-      </c>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+        <v>efc9d2dd-368d-012b-28f4-a55bb62e851f</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8726,10 +8726,10 @@
       </c>
       <c r="W100" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>ff30d137-83b8-753a-660d-bad60ea9a014</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+        <v>20aa3ecb-1d39-4140-0a34-e7b48fa78a57</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8794,10 +8794,10 @@
       </c>
       <c r="W101" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>8e002996-0b74-2e25-0e8d-a25176dd3935</v>
-      </c>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+        <v>9df353da-6e39-08f7-a6d4-e15c2d474a16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8861,7 +8861,7 @@
         <v>&lt;value102&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483763&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro101&lt;/name&gt; &lt;id&gt;{c7b6a901-56af-0fe1-4456-74be42cb2c7b}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;International1&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value102&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8925,7 +8925,7 @@
         <v>&lt;value103&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483764&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro102&lt;/name&gt; &lt;id&gt;{6e20b69c-0634-08ec-3bf7-1f437b9a956a}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;International1&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value103&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -8989,7 +8989,7 @@
         <v>&lt;value104&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483765&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro103&lt;/name&gt; &lt;id&gt;{25297473-6175-5f9b-85c7-2ccd0a6662d8}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International1&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value104&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -9053,7 +9053,7 @@
         <v>&lt;value105&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483766&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro104&lt;/name&gt; &lt;id&gt;{c421be72-4f95-a21e-9cf4-7785cfdd216c}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;International1&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value105&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -9118,7 +9118,7 @@
         <v>&lt;value106&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483767&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro105&lt;/name&gt; &lt;id&gt;{512fd651-1e4e-3a51-2154-7905ff8c2f16}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;International2&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value106&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="str">
         <f t="shared" si="163"/>
         <v>&lt;value</v>
@@ -9183,13 +9183,13 @@
         <v>&lt;value107&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483768&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro106&lt;/name&gt; &lt;id&gt;{0aebfa9c-a428-14bf-616c-f9f7f592906b}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;International2&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value107&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="str">
-        <f t="shared" ref="A108:A113" si="224">A107</f>
+        <f t="shared" ref="A108:A144" si="224">A107</f>
         <v>&lt;value</v>
       </c>
       <c r="B108">
-        <f t="shared" ref="B108:B113" si="225">B107+1</f>
+        <f t="shared" ref="B108:B144" si="225">B107+1</f>
         <v>108</v>
       </c>
       <c r="C108" s="1" t="str">
@@ -9197,14 +9197,14 @@
         <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
       </c>
       <c r="D108">
-        <f t="shared" ref="D108:D113" si="226">D107+1</f>
+        <f t="shared" ref="D108:D144" si="226">D107+1</f>
         <v>2147483769</v>
       </c>
       <c r="E108" t="s">
         <v>48</v>
       </c>
       <c r="F108">
-        <f t="shared" ref="F108:F113" si="227">F107+1</f>
+        <f t="shared" ref="F108:F144" si="227">F107+1</f>
         <v>107</v>
       </c>
       <c r="G108" t="s">
@@ -9214,7 +9214,7 @@
         <v>160</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f t="shared" ref="I108:I113" si="228">I107</f>
+        <f t="shared" ref="I108:I144" si="228">I107</f>
         <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -9248,7 +9248,7 @@
         <v>&lt;value108&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483769&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro107&lt;/name&gt; &lt;id&gt;{be4e1a2c-55b2-2aed-443c-d8fec9fa3a9f}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;International2&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value108&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="str">
         <f t="shared" si="224"/>
         <v>&lt;value</v>
@@ -9313,7 +9313,7 @@
         <v>&lt;value109&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483770&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro108&lt;/name&gt; &lt;id&gt;{78c46af1-087d-4c48-7bfd-3a59e4499262}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International2&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value109&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="str">
         <f t="shared" si="224"/>
         <v>&lt;value</v>
@@ -9378,7 +9378,7 @@
         <v>&lt;value110&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483771&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro109&lt;/name&gt; &lt;id&gt;{21ecee52-2298-3b4b-6b32-dc49481c407c}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;International2&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value110&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="str">
         <f t="shared" si="224"/>
         <v>&lt;value</v>
@@ -9443,7 +9443,7 @@
         <v>&lt;value111&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483772&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro110&lt;/name&gt; &lt;id&gt;{b2b97ce2-797d-3676-4123-89c5570d1f42}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;International2&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value111&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="str">
         <f t="shared" si="224"/>
         <v>&lt;value</v>
@@ -9508,7 +9508,7 @@
         <v>&lt;value112&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483773&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro111&lt;/name&gt; &lt;id&gt;{a1a89805-1401-896e-90fe-b839bd9b8665}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International2&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value112&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="str">
         <f t="shared" si="224"/>
         <v>&lt;value</v>
@@ -9543,7 +9543,7 @@
         <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
       </c>
       <c r="J113" s="1" t="str">
-        <f t="shared" ref="J113" si="241">J105</f>
+        <f t="shared" ref="J113:J144" si="241">J105</f>
         <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;</v>
       </c>
       <c r="K113" s="1" t="str">
@@ -9551,7 +9551,7 @@
         <v>International2</v>
       </c>
       <c r="L113" s="1" t="str">
-        <f t="shared" ref="L113" si="242">L105</f>
+        <f t="shared" ref="L113:L144" si="242">L105</f>
         <v>&lt;/value3&gt;</v>
       </c>
       <c r="M113" t="s">
@@ -9572,6 +9572,1181 @@
         <f t="shared" si="135"/>
         <v>&lt;value113&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483774&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro112&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;International2&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value113&gt;</v>
       </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="225"/>
+        <v>114</v>
+      </c>
+      <c r="C114" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="226"/>
+        <v>2147483775</v>
+      </c>
+      <c r="E114" t="s">
+        <v>48</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="227"/>
+        <v>113</v>
+      </c>
+      <c r="G114" t="s">
+        <v>47</v>
+      </c>
+      <c r="H114" t="s">
+        <v>165</v>
+      </c>
+      <c r="I114" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J114" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;</v>
+      </c>
+      <c r="K114" s="1" t="str">
+        <f t="shared" ref="K114:K144" si="243">_xlfn.CONCAT("International", Q114)</f>
+        <v>International3</v>
+      </c>
+      <c r="L114" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value0&gt;</v>
+      </c>
+      <c r="M114" t="s">
+        <v>27</v>
+      </c>
+      <c r="N114">
+        <f t="shared" ref="N114:N144" si="244">B114</f>
+        <v>114</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q114">
+        <f>Q106+1</f>
+        <v>3</v>
+      </c>
+      <c r="T114" s="3" t="str">
+        <f t="shared" ref="T114:T144" si="245">_xlfn.CONCAT(A114:O114)</f>
+        <v>&lt;value114&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483775&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro113&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;International3&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value114&gt;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="225"/>
+        <v>115</v>
+      </c>
+      <c r="C115" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="226"/>
+        <v>2147483776</v>
+      </c>
+      <c r="E115" t="s">
+        <v>48</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="227"/>
+        <v>114</v>
+      </c>
+      <c r="G115" t="s">
+        <v>47</v>
+      </c>
+      <c r="H115" t="s">
+        <v>165</v>
+      </c>
+      <c r="I115" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J115" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K115" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L115" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M115" t="s">
+        <v>27</v>
+      </c>
+      <c r="N115">
+        <f t="shared" si="244"/>
+        <v>115</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q115">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T115" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value115&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483776&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro114&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;International3&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value115&gt;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="225"/>
+        <v>116</v>
+      </c>
+      <c r="C116" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="226"/>
+        <v>2147483777</v>
+      </c>
+      <c r="E116" t="s">
+        <v>48</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="227"/>
+        <v>115</v>
+      </c>
+      <c r="G116" t="s">
+        <v>47</v>
+      </c>
+      <c r="H116" t="s">
+        <v>165</v>
+      </c>
+      <c r="I116" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J116" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K116" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L116" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M116" t="s">
+        <v>27</v>
+      </c>
+      <c r="N116">
+        <f t="shared" si="244"/>
+        <v>116</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q116">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T116" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value116&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483777&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro115&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;International3&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value116&gt;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="225"/>
+        <v>117</v>
+      </c>
+      <c r="C117" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="226"/>
+        <v>2147483778</v>
+      </c>
+      <c r="E117" t="s">
+        <v>48</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="227"/>
+        <v>116</v>
+      </c>
+      <c r="G117" t="s">
+        <v>47</v>
+      </c>
+      <c r="H117" t="s">
+        <v>165</v>
+      </c>
+      <c r="I117" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J117" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K117" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L117" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M117" t="s">
+        <v>27</v>
+      </c>
+      <c r="N117">
+        <f t="shared" si="244"/>
+        <v>117</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q117">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T117" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value117&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483778&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro116&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International3&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value117&gt;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="225"/>
+        <v>118</v>
+      </c>
+      <c r="C118" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="226"/>
+        <v>2147483779</v>
+      </c>
+      <c r="E118" t="s">
+        <v>48</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="227"/>
+        <v>117</v>
+      </c>
+      <c r="G118" t="s">
+        <v>47</v>
+      </c>
+      <c r="H118" t="s">
+        <v>165</v>
+      </c>
+      <c r="I118" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J118" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K118" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L118" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M118" t="s">
+        <v>27</v>
+      </c>
+      <c r="N118">
+        <f t="shared" si="244"/>
+        <v>118</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q118">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T118" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value118&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483779&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro117&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;International3&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value118&gt;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="225"/>
+        <v>119</v>
+      </c>
+      <c r="C119" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="226"/>
+        <v>2147483780</v>
+      </c>
+      <c r="E119" t="s">
+        <v>48</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="227"/>
+        <v>118</v>
+      </c>
+      <c r="G119" t="s">
+        <v>47</v>
+      </c>
+      <c r="H119" t="s">
+        <v>165</v>
+      </c>
+      <c r="I119" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J119" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K119" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L119" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M119" t="s">
+        <v>27</v>
+      </c>
+      <c r="N119">
+        <f t="shared" si="244"/>
+        <v>119</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q119">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T119" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value119&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483780&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro118&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;International3&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value119&gt;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="225"/>
+        <v>120</v>
+      </c>
+      <c r="C120" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="226"/>
+        <v>2147483781</v>
+      </c>
+      <c r="E120" t="s">
+        <v>48</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="227"/>
+        <v>119</v>
+      </c>
+      <c r="G120" t="s">
+        <v>47</v>
+      </c>
+      <c r="H120" t="s">
+        <v>165</v>
+      </c>
+      <c r="I120" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J120" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K120" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L120" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M120" t="s">
+        <v>27</v>
+      </c>
+      <c r="N120">
+        <f t="shared" si="244"/>
+        <v>120</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q120">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T120" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value120&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483781&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro119&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International3&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value120&gt;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="225"/>
+        <v>121</v>
+      </c>
+      <c r="C121" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="226"/>
+        <v>2147483782</v>
+      </c>
+      <c r="E121" t="s">
+        <v>48</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="227"/>
+        <v>120</v>
+      </c>
+      <c r="G121" t="s">
+        <v>47</v>
+      </c>
+      <c r="H121" t="s">
+        <v>165</v>
+      </c>
+      <c r="I121" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J121" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;</v>
+      </c>
+      <c r="K121" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International3</v>
+      </c>
+      <c r="L121" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value3&gt;</v>
+      </c>
+      <c r="M121" t="s">
+        <v>27</v>
+      </c>
+      <c r="N121">
+        <f t="shared" si="244"/>
+        <v>121</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q121">
+        <f t="shared" si="150"/>
+        <v>3</v>
+      </c>
+      <c r="T121" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value121&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483782&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro120&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;International3&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value121&gt;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="225"/>
+        <v>122</v>
+      </c>
+      <c r="C122" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="226"/>
+        <v>2147483783</v>
+      </c>
+      <c r="E122" t="s">
+        <v>48</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="227"/>
+        <v>121</v>
+      </c>
+      <c r="G122" t="s">
+        <v>47</v>
+      </c>
+      <c r="H122" t="s">
+        <v>165</v>
+      </c>
+      <c r="I122" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J122" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;</v>
+      </c>
+      <c r="K122" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L122" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value0&gt;</v>
+      </c>
+      <c r="M122" t="s">
+        <v>27</v>
+      </c>
+      <c r="N122">
+        <f t="shared" si="244"/>
+        <v>122</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q122">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T122" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value122&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483783&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro121&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;International4&lt;/value0&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value122&gt;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="225"/>
+        <v>123</v>
+      </c>
+      <c r="C123" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="226"/>
+        <v>2147483784</v>
+      </c>
+      <c r="E123" t="s">
+        <v>48</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="227"/>
+        <v>122</v>
+      </c>
+      <c r="G123" t="s">
+        <v>47</v>
+      </c>
+      <c r="H123" t="s">
+        <v>165</v>
+      </c>
+      <c r="I123" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J123" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K123" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L123" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M123" t="s">
+        <v>27</v>
+      </c>
+      <c r="N123">
+        <f t="shared" si="244"/>
+        <v>123</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q123">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T123" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value123&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483784&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro122&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;International4&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value123&gt;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="225"/>
+        <v>124</v>
+      </c>
+      <c r="C124" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="226"/>
+        <v>2147483785</v>
+      </c>
+      <c r="E124" t="s">
+        <v>48</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="227"/>
+        <v>123</v>
+      </c>
+      <c r="G124" t="s">
+        <v>47</v>
+      </c>
+      <c r="H124" t="s">
+        <v>165</v>
+      </c>
+      <c r="I124" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J124" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K124" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L124" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M124" t="s">
+        <v>27</v>
+      </c>
+      <c r="N124">
+        <f t="shared" si="244"/>
+        <v>124</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q124">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T124" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value124&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483785&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro123&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftAlt&lt;/value0&gt; &lt;value1&gt;International4&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value124&gt;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="225"/>
+        <v>125</v>
+      </c>
+      <c r="C125" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="226"/>
+        <v>2147483786</v>
+      </c>
+      <c r="E125" t="s">
+        <v>48</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="227"/>
+        <v>124</v>
+      </c>
+      <c r="G125" t="s">
+        <v>47</v>
+      </c>
+      <c r="H125" t="s">
+        <v>165</v>
+      </c>
+      <c r="I125" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J125" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K125" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L125" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M125" t="s">
+        <v>27</v>
+      </c>
+      <c r="N125">
+        <f t="shared" si="244"/>
+        <v>125</v>
+      </c>
+      <c r="O125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q125">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T125" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value125&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483786&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro124&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International4&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value125&gt;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="225"/>
+        <v>126</v>
+      </c>
+      <c r="C126" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="226"/>
+        <v>2147483787</v>
+      </c>
+      <c r="E126" t="s">
+        <v>48</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="227"/>
+        <v>125</v>
+      </c>
+      <c r="G126" t="s">
+        <v>47</v>
+      </c>
+      <c r="H126" t="s">
+        <v>165</v>
+      </c>
+      <c r="I126" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J126" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;</v>
+      </c>
+      <c r="K126" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L126" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value1&gt;</v>
+      </c>
+      <c r="M126" t="s">
+        <v>27</v>
+      </c>
+      <c r="N126">
+        <f t="shared" si="244"/>
+        <v>126</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q126">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T126" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value126&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483787&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro125&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;International4&lt;/value1&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value126&gt;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="225"/>
+        <v>127</v>
+      </c>
+      <c r="C127" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="226"/>
+        <v>2147483788</v>
+      </c>
+      <c r="E127" t="s">
+        <v>48</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="227"/>
+        <v>126</v>
+      </c>
+      <c r="G127" t="s">
+        <v>47</v>
+      </c>
+      <c r="H127" t="s">
+        <v>165</v>
+      </c>
+      <c r="I127" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J127" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K127" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L127" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M127" t="s">
+        <v>27</v>
+      </c>
+      <c r="N127">
+        <f t="shared" si="244"/>
+        <v>127</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T127" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value127&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483788&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro126&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;International4&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value127&gt;</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="225"/>
+        <v>128</v>
+      </c>
+      <c r="C128" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="226"/>
+        <v>2147483789</v>
+      </c>
+      <c r="E128" t="s">
+        <v>48</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="227"/>
+        <v>127</v>
+      </c>
+      <c r="G128" t="s">
+        <v>47</v>
+      </c>
+      <c r="H128" t="s">
+        <v>165</v>
+      </c>
+      <c r="I128" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J128" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;</v>
+      </c>
+      <c r="K128" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L128" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value2&gt;</v>
+      </c>
+      <c r="M128" t="s">
+        <v>27</v>
+      </c>
+      <c r="N128">
+        <f t="shared" si="244"/>
+        <v>128</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q128">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T128" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value128&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483789&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro127&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftShift&lt;/value0&gt; &lt;value1&gt;LeftAlt&lt;/value1&gt; &lt;value2&gt;International4&lt;/value2&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value128&gt;</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="str">
+        <f t="shared" si="224"/>
+        <v>&lt;value</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="225"/>
+        <v>129</v>
+      </c>
+      <c r="C129" s="1" t="str">
+        <f t="shared" si="165"/>
+        <v>&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="226"/>
+        <v>2147483790</v>
+      </c>
+      <c r="E129" t="s">
+        <v>48</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="227"/>
+        <v>128</v>
+      </c>
+      <c r="G129" t="s">
+        <v>47</v>
+      </c>
+      <c r="H129" t="s">
+        <v>165</v>
+      </c>
+      <c r="I129" s="1" t="str">
+        <f t="shared" si="228"/>
+        <v>}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;</v>
+      </c>
+      <c r="J129" s="1" t="str">
+        <f t="shared" si="241"/>
+        <v>&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;</v>
+      </c>
+      <c r="K129" s="1" t="str">
+        <f t="shared" si="243"/>
+        <v>International4</v>
+      </c>
+      <c r="L129" s="1" t="str">
+        <f t="shared" si="242"/>
+        <v>&lt;/value3&gt;</v>
+      </c>
+      <c r="M129" t="s">
+        <v>27</v>
+      </c>
+      <c r="N129">
+        <f t="shared" si="244"/>
+        <v>129</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q129">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="T129" s="3" t="str">
+        <f t="shared" si="245"/>
+        <v>&lt;value129&gt; &lt;first&gt; &lt;polymorphic_id&gt;27&lt;/polymorphic_id&gt; &lt;ptr_wrapper&gt; &lt;id&gt;2147483790&lt;/id&gt; &lt;data&gt; &lt;base&gt; &lt;name&gt;PowerAppsMainMacro128&lt;/name&gt; &lt;id&gt;{a0028502-9c88-9e1f-1be0-4e8897b789d4}&lt;/id&gt;&lt;repeatOptions&gt; &lt;repeatCount&gt;1&lt;/repeatCount&gt; &lt;repeatMode&gt;NoRepeat&lt;/repeatMode&gt; &lt;delay&gt;0&lt;/delay&gt; &lt;delayMode&gt;Constant&lt;/delayMode&gt; &lt;randomDelayFrom&gt;0&lt;/randomDelayFrom&gt; &lt;randomDelayTo&gt;0&lt;/randomDelayTo&gt; &lt;/repeatOptions&gt;&lt;executionHints&gt; &lt;terminateOnSecondExec&gt;false&lt;/terminateOnSecondExec&gt; &lt;restartOnSecondExec&gt;false&lt;/restartOnSecondExec&gt; &lt;execHint&gt;OnBoth&lt;/execHint&gt; &lt;retainOriginalKeyOutput&gt;false&lt;/retainOriginalKeyOutput&gt; &lt;/executionHints&gt;&lt;actionLighting&gt;{00000000-0000-0000-0000-000000000000}&lt;/actionLighting&gt;&lt;actionSoundPath&gt;&lt;/actionSoundPath&gt;&lt;attachedActions size="dynamic" /&gt;&lt;/base&gt;&lt;keyName&gt;&lt;/keyName&gt;&lt;keyStroke size="dynamic"&gt;&lt;value0&gt;LeftCtrl&lt;/value0&gt; &lt;value1&gt;LeftShift&lt;/value1&gt; &lt;value2&gt;LeftAlt&lt;/value2&gt; &lt;value3&gt;International4&lt;/value3&gt;&lt;/keyStroke&gt;&lt;holdingKeyEnabled&gt;false&lt;/holdingKeyEnabled&gt;&lt;holdingKeyType&gt;OnPress&lt;/holdingKeyType&gt;&lt;holdingKeyOnPressInterval&gt;100&lt;/holdingKeyOnPressInterval&gt;&lt;sniperSwitchMode&gt;WhilePressed&lt;/sniperSwitchMode&gt;&lt;/data&gt;&lt;/ptr_wrapper&gt;&lt;/first&gt;&lt;second&gt; &lt;first&gt;F1&lt;/first&gt; &lt;second&gt;Click&lt;/second&gt; &lt;/second&gt;&lt;/value129&gt;</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="O130" s="1"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="O131" s="1"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="O132" s="1"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="O133" s="1"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="O134" s="1"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="O135" s="1"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="O136" s="1"/>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="O137" s="1"/>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="O138" s="1"/>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="O139" s="1"/>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="O140" s="1"/>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="O141" s="1"/>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="O142" s="1"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="O143" s="1"/>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="O144" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9583,20 +10758,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E279DDDB-1CE1-4893-A52C-DF2DBA95B302}">
   <dimension ref="A1:V113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -9628,7 +10803,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9688,7 +10863,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -10200,7 +11375,7 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A10" si="5">A3+1</f>
         <v>3</v>
@@ -10257,7 +11432,7 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -10314,7 +11489,7 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -10371,7 +11546,7 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -10428,7 +11603,7 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -10485,7 +11660,7 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -10542,7 +11717,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -10599,7 +11774,7 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ref="A11:A74" si="8">A10+1</f>
         <v>10</v>
@@ -10656,7 +11831,7 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -10713,7 +11888,7 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -10770,7 +11945,7 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="8"/>
         <v>13</v>
@@ -10827,7 +12002,7 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="8"/>
         <v>14</v>
@@ -10884,7 +12059,7 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -10941,7 +12116,7 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="8"/>
         <v>16</v>
@@ -10998,7 +12173,7 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -11055,7 +12230,7 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -11112,7 +12287,7 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -11169,7 +12344,7 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -11226,7 +12401,7 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -11283,7 +12458,7 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -11340,7 +12515,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -11397,7 +12572,7 @@
 </v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -11454,7 +12629,7 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -11511,7 +12686,7 @@
 </v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="8"/>
         <v>26</v>
@@ -11568,7 +12743,7 @@
 </v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="8"/>
         <v>27</v>
@@ -11625,7 +12800,7 @@
 </v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="8"/>
         <v>28</v>
@@ -11682,7 +12857,7 @@
 </v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -11739,7 +12914,7 @@
 </v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="8"/>
         <v>30</v>
@@ -11796,7 +12971,7 @@
 </v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>31</v>
@@ -11853,7 +13028,7 @@
 </v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="8"/>
         <v>32</v>
@@ -11910,7 +13085,7 @@
 </v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="8"/>
         <v>33</v>
@@ -11967,7 +13142,7 @@
 </v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>34</v>
@@ -12024,7 +13199,7 @@
 </v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>35</v>
@@ -12081,7 +13256,7 @@
 </v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>36</v>
@@ -12138,7 +13313,7 @@
 </v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>37</v>
@@ -12195,7 +13370,7 @@
 </v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>38</v>
@@ -12252,7 +13427,7 @@
 </v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>39</v>
@@ -12309,7 +13484,7 @@
 </v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="8"/>
         <v>40</v>
@@ -12366,7 +13541,7 @@
 </v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="8"/>
         <v>41</v>
@@ -12423,7 +13598,7 @@
 </v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="8"/>
         <v>42</v>
@@ -12480,7 +13655,7 @@
 </v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="8"/>
         <v>43</v>
@@ -12537,7 +13712,7 @@
 </v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="8"/>
         <v>44</v>
@@ -12594,7 +13769,7 @@
 </v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="8"/>
         <v>45</v>
@@ -12651,7 +13826,7 @@
 </v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="8"/>
         <v>46</v>
@@ -12708,7 +13883,7 @@
 </v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="8"/>
         <v>47</v>
@@ -12765,7 +13940,7 @@
 </v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="8"/>
         <v>48</v>
@@ -12822,7 +13997,7 @@
 </v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="8"/>
         <v>49</v>
@@ -12879,7 +14054,7 @@
 </v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="8"/>
         <v>50</v>
@@ -12936,7 +14111,7 @@
 </v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="8"/>
         <v>51</v>
@@ -12993,7 +14168,7 @@
 </v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="8"/>
         <v>52</v>
@@ -13050,7 +14225,7 @@
 </v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="8"/>
         <v>53</v>
@@ -13107,7 +14282,7 @@
 </v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="8"/>
         <v>54</v>
@@ -13164,7 +14339,7 @@
 </v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="8"/>
         <v>55</v>
@@ -13221,7 +14396,7 @@
 </v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="8"/>
         <v>56</v>
@@ -13278,7 +14453,7 @@
 </v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="8"/>
         <v>57</v>
@@ -13335,7 +14510,7 @@
 </v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="8"/>
         <v>58</v>
@@ -13392,7 +14567,7 @@
 </v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="8"/>
         <v>59</v>
@@ -13449,7 +14624,7 @@
 </v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="8"/>
         <v>60</v>
@@ -13506,7 +14681,7 @@
 </v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="8"/>
         <v>61</v>
@@ -13563,7 +14738,7 @@
 </v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="8"/>
         <v>62</v>
@@ -13620,7 +14795,7 @@
 </v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="8"/>
         <v>63</v>
@@ -13677,7 +14852,7 @@
 </v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="8"/>
         <v>64</v>
@@ -13734,7 +14909,7 @@
 </v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="8"/>
         <v>65</v>
@@ -13791,7 +14966,7 @@
 </v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="8"/>
         <v>66</v>
@@ -13848,7 +15023,7 @@
 </v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="8"/>
         <v>67</v>
@@ -13905,7 +15080,7 @@
 </v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="8"/>
         <v>68</v>
@@ -13962,7 +15137,7 @@
 </v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="8"/>
         <v>69</v>
@@ -14019,7 +15194,7 @@
 </v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="8"/>
         <v>70</v>
@@ -14076,7 +15251,7 @@
 </v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="8"/>
         <v>71</v>
@@ -14133,7 +15308,7 @@
 </v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="8"/>
         <v>72</v>
@@ -14190,7 +15365,7 @@
 </v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="8"/>
         <v>73</v>
@@ -14247,7 +15422,7 @@
 </v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" ref="A75:A112" si="16">A74+1</f>
         <v>74</v>
@@ -14304,7 +15479,7 @@
 </v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="16"/>
         <v>75</v>
@@ -14361,7 +15536,7 @@
 </v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="16"/>
         <v>76</v>
@@ -14418,7 +15593,7 @@
 </v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="16"/>
         <v>77</v>
@@ -14475,7 +15650,7 @@
 </v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="16"/>
         <v>78</v>
@@ -14532,7 +15707,7 @@
 </v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="16"/>
         <v>79</v>
@@ -14589,7 +15764,7 @@
 </v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="16"/>
         <v>80</v>
@@ -14646,7 +15821,7 @@
 </v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="16"/>
         <v>81</v>
@@ -14703,7 +15878,7 @@
 </v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="16"/>
         <v>82</v>
@@ -14760,7 +15935,7 @@
 </v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="16"/>
         <v>83</v>
@@ -14817,7 +15992,7 @@
 </v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="16"/>
         <v>84</v>
@@ -14874,7 +16049,7 @@
 </v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="16"/>
         <v>85</v>
@@ -14931,7 +16106,7 @@
 </v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="16"/>
         <v>86</v>
@@ -14988,7 +16163,7 @@
 </v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="16"/>
         <v>87</v>
@@ -15045,7 +16220,7 @@
 </v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="16"/>
         <v>88</v>
@@ -15102,7 +16277,7 @@
 </v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="16"/>
         <v>89</v>
@@ -15159,7 +16334,7 @@
 </v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="16"/>
         <v>90</v>
@@ -15216,7 +16391,7 @@
 </v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="16"/>
         <v>91</v>
@@ -15273,7 +16448,7 @@
 </v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="16"/>
         <v>92</v>
@@ -15330,7 +16505,7 @@
 </v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="16"/>
         <v>93</v>
@@ -15387,7 +16562,7 @@
 </v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="16"/>
         <v>94</v>
@@ -15444,7 +16619,7 @@
 </v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="16"/>
         <v>95</v>
@@ -15501,7 +16676,7 @@
 </v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="16"/>
         <v>96</v>
@@ -15558,7 +16733,7 @@
 </v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="16"/>
         <v>97</v>
@@ -15614,7 +16789,7 @@
 </v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="16"/>
         <v>98</v>
@@ -15670,7 +16845,7 @@
 </v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="16"/>
         <v>99</v>
@@ -15726,7 +16901,7 @@
 </v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="16"/>
         <v>100</v>
@@ -15782,7 +16957,7 @@
 </v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <f t="shared" si="16"/>
         <v>101</v>
@@ -15838,7 +17013,7 @@
 </v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <f t="shared" si="16"/>
         <v>102</v>
@@ -15894,7 +17069,7 @@
 </v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <f t="shared" si="16"/>
         <v>103</v>
@@ -15950,7 +17125,7 @@
 </v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <f t="shared" si="16"/>
         <v>104</v>
@@ -16006,7 +17181,7 @@
 </v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <f t="shared" si="16"/>
         <v>105</v>
@@ -16062,7 +17237,7 @@
 </v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <f t="shared" si="16"/>
         <v>106</v>
@@ -16118,7 +17293,7 @@
 </v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <f t="shared" si="16"/>
         <v>107</v>
@@ -16168,7 +17343,7 @@
 </v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <f t="shared" si="16"/>
         <v>108</v>
@@ -16218,7 +17393,7 @@
 </v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <f t="shared" si="16"/>
         <v>109</v>
@@ -16268,7 +17443,7 @@
 </v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <f t="shared" si="16"/>
         <v>110</v>
@@ -16318,7 +17493,7 @@
 </v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <f t="shared" si="16"/>
         <v>111</v>
@@ -16368,7 +17543,7 @@
 </v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <f t="shared" ref="A113" si="24">A112+1</f>
         <v>112</v>
@@ -16433,9 +17608,9 @@
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:26" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
         <v>288</v>
       </c>
@@ -16461,7 +17636,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
         <v>296</v>
       </c>
@@ -16514,7 +17689,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
         <v>313</v>
       </c>
@@ -16567,7 +17742,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.3">
       <c r="G8" t="s">
         <v>328</v>
       </c>
@@ -16599,7 +17774,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>336</v>
       </c>
@@ -16628,17 +17803,17 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>345</v>
       </c>
@@ -16646,12 +17821,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.3">
       <c r="G16" s="5" t="s">
         <v>16</v>
       </c>
@@ -16662,7 +17837,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="7:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:22" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>350</v>
       </c>
@@ -16673,7 +17848,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="7:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:22" x14ac:dyDescent="0.3">
       <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
@@ -16684,7 +17859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="7:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:22" x14ac:dyDescent="0.3">
       <c r="G20" t="s">
         <v>354</v>
       </c>
@@ -16708,9 +17883,9 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -16730,7 +17905,7 @@
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
     </row>
-    <row r="2" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>364</v>
@@ -16766,7 +17941,7 @@
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
     </row>
-    <row r="3" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -16786,7 +17961,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -16806,7 +17981,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -16826,7 +18001,7 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="10"/>
     </row>
-    <row r="6" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>296</v>
       </c>
@@ -16868,7 +18043,7 @@
       <c r="Q6" s="14"/>
       <c r="R6" s="10"/>
     </row>
-    <row r="7" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>313</v>
       </c>
@@ -16910,7 +18085,7 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="10"/>
     </row>
-    <row r="8" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>328</v>
       </c>
@@ -16950,7 +18125,7 @@
       <c r="Q8" s="14"/>
       <c r="R8" s="10"/>
     </row>
-    <row r="9" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>336</v>
       </c>
@@ -16988,7 +18163,7 @@
       <c r="Q9" s="14"/>
       <c r="R9" s="10"/>
     </row>
-    <row r="10" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -17000,7 +18175,7 @@
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
     </row>
-    <row r="11" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -17030,7 +18205,7 @@
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
     </row>
-    <row r="12" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -17062,7 +18237,7 @@
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
@@ -17086,7 +18261,7 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
     </row>
-    <row r="14" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
@@ -17110,7 +18285,7 @@
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
     </row>
-    <row r="15" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -17132,7 +18307,7 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
     </row>
-    <row r="16" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -17156,7 +18331,7 @@
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
     </row>
-    <row r="17" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
         <v>343</v>
@@ -17188,7 +18363,7 @@
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
     </row>
-    <row r="18" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
         <v>344</v>
@@ -17216,7 +18391,7 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -17236,7 +18411,7 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -17253,31 +18428,31 @@
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:18" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:18" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>